<commit_message>
Delete old shift template
</commit_message>
<xml_diff>
--- a/templates/accupay-shiftschedule-template.xlsx
+++ b/templates/accupay-shiftschedule-template.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
-    <sheet name="SAMPLE" sheetId="3" r:id="rId2"/>
+    <sheet name="EXAMPLE" sheetId="3" r:id="rId2"/>
     <sheet name="Employee Shift" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -21,7 +21,7 @@
     <t>AccuPay Shift Schedule Template</t>
   </si>
   <si>
-    <t>In this file, you will set your employees' shift schedule for the whole month, pay period or whatever length you desire. To use, just add the supply the information in the columns provided.</t>
+    <t>In this file, you will set your employees' shift schedule for the whole month, pay period or whatever length you desire. To use, just supply the information in the columns provided.</t>
   </si>
   <si>
     <t>Legend</t>
@@ -48,13 +48,13 @@
     <t>`Effective Date From`</t>
   </si>
   <si>
-    <t>The date to which the shift will apply</t>
+    <t>The date to which the shift will first apply</t>
   </si>
   <si>
     <t>`Effective Date To`</t>
   </si>
   <si>
-    <t>The last date the shift will apply</t>
+    <t>The last date the shift will apply (optional)</t>
   </si>
   <si>
     <t>`Schedule Type`</t>
@@ -63,19 +63,13 @@
     <t>Leave blank</t>
   </si>
   <si>
-    <t>Note: Refer to the worksheet `SAMPLE` for an example.</t>
-  </si>
-  <si>
-    <t>Note: Use the blank worksheet `Employee Shift` to add your shifts</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
+    <t>NOTE: Refer to the worksheet `EXAMPLE` for an example.</t>
+  </si>
+  <si>
+    <t>NOTE: Use the blank worksheet `Employee Shift` to add your shifts</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">In this example, we are giving employe </t>
     </r>
     <r>
@@ -219,7 +213,7 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>1/9/2017</t>
+      <t>1/1/2017</t>
     </r>
     <r>
       <rPr>
@@ -294,9 +288,9 @@
     <numFmt numFmtId="176" formatCode="h:mm;@"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="180" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="26">
@@ -342,6 +336,105 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -351,65 +444,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -417,70 +451,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -502,18 +496,180 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -521,168 +677,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -698,8 +692,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -735,6 +731,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -753,8 +767,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -773,30 +787,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -814,130 +808,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1344,7 +1338,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1512,7 +1506,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1618,17 +1612,15 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="13.8571428571429" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1428571428571" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.1428571428571" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.7142857142857" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.1428571428571" style="3" customWidth="1"/>
-    <col min="6" max="6" width="14" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" style="1" customWidth="1"/>
+    <col min="2" max="3" width="12.7142857142857" style="2" customWidth="1"/>
+    <col min="4" max="5" width="18.7142857142857" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.7142857142857" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>